<commit_message>
Update example input files to include Dp
</commit_message>
<xml_diff>
--- a/Shiny-IEX/Examples/example_input_medium.xlsx
+++ b/Shiny-IEX/Examples/example_input_medium.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/sandlin_cole_epa_gov/Documents/Profile/Documents/GitHub/Water_Treatment_Models/Shiny-IEX/Examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{E252C32D-DBEC-4A19-859C-D1F86BD654B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CE126D1-F0A7-425E-A1CF-8ED5AC632608}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{E252C32D-DBEC-4A19-859C-D1F86BD654B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3C5ED74-057B-4955-86D6-B064FBD34849}"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="1480" windowWidth="14400" windowHeight="7270" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="39">
   <si>
     <t>name</t>
   </si>
@@ -144,6 +144,12 @@
   </si>
   <si>
     <t>ng</t>
+  </si>
+  <si>
+    <t>Dp</t>
+  </si>
+  <si>
+    <t>Dp_units</t>
   </si>
 </sst>
 </file>
@@ -215,9 +221,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -255,7 +261,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -361,7 +367,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -503,7 +509,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -513,9 +519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -644,18 +648,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6:I10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -681,10 +683,16 @@
         <v>26</v>
       </c>
       <c r="I1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -709,11 +717,17 @@
       <c r="H2" t="s">
         <v>35</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -738,11 +752,17 @@
       <c r="H3" t="s">
         <v>35</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="1">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="J3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -767,11 +787,17 @@
       <c r="H4" t="s">
         <v>35</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="1">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="J4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -796,11 +822,17 @@
       <c r="H5" t="s">
         <v>35</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="1">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="J5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -825,11 +857,17 @@
       <c r="H6" t="s">
         <v>35</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="1">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="J6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -854,11 +892,17 @@
       <c r="H7" t="s">
         <v>35</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="1">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="J7" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -883,11 +927,17 @@
       <c r="H8" t="s">
         <v>35</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="1">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="J8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -912,11 +962,17 @@
       <c r="H9" t="s">
         <v>35</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="1">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="J9" t="s">
+        <v>35</v>
+      </c>
+      <c r="K9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -941,7 +997,13 @@
       <c r="H10" t="s">
         <v>35</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="1">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="J10" t="s">
+        <v>35</v>
+      </c>
+      <c r="K10" t="s">
         <v>36</v>
       </c>
     </row>
@@ -955,9 +1017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>

</xml_diff>